<commit_message>
Aggiornato data.json con caso id 37; Aggiornato il report; Caricato il pdf del caso id 37
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -231,6 +231,12 @@
     </r>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Il caso di test non è applicabile poiché il token JWT può contenere campi valorizzati in maniera errata ma comunque sempre presenti</t>
+  </si>
+  <si>
     <t>KO</t>
   </si>
   <si>
@@ -294,11 +300,32 @@
     </r>
   </si>
   <si>
+    <t>11:01:00</t>
+  </si>
+  <si>
+    <t>8c463e33a4928d82</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.44cc2c90f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>JWT payload: Tipologia documento diversa dalla tipologia di CDA (code - codesystem)</t>
+  </si>
+  <si>
+    <t>L’applicativo risponde con un codice di errore e il messaggio “Campo token JWT non valido” seguito dal motivo dell’errore. Il referto non viene prodotto</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_LDO_TIMEOUT</t>
   </si>
   <si>
     <t xml:space="preserve">
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
+  </si>
+  <si>
+    <t>11:03:00</t>
+  </si>
+  <si>
+    <t>In caso di timeout con il gateway il processo clinico prosegue, il referto viene prodotto</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -307,9 +334,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>Il software non consente che per un paziente non sia presente il codice fiscale</t>
@@ -825,7 +849,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -841,6 +865,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -931,21 +970,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -965,7 +989,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1092,37 +1116,49 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1152,22 +1188,22 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1176,19 +1212,19 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2766,8 +2802,12 @@
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="37"/>
+      <c r="J14" t="s" s="36">
+        <v>47</v>
+      </c>
+      <c r="K14" t="s" s="42">
+        <v>48</v>
+      </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="37"/>
@@ -2777,7 +2817,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="39"/>
       <c r="T14" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" ht="105.55" customHeight="1">
@@ -2791,30 +2831,50 @@
         <v>27</v>
       </c>
       <c r="D15" t="s" s="31">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s" s="41">
-        <v>49</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="37"/>
+        <v>51</v>
+      </c>
+      <c r="F15" s="33">
+        <v>44991</v>
+      </c>
+      <c r="G15" t="s" s="35">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s" s="35">
+        <v>53</v>
+      </c>
+      <c r="I15" t="s" s="35">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s" s="36">
+        <v>32</v>
+      </c>
+      <c r="K15" s="43"/>
+      <c r="L15" t="s" s="36">
+        <v>32</v>
+      </c>
+      <c r="M15" t="s" s="36">
+        <v>47</v>
+      </c>
+      <c r="N15" t="s" s="44">
+        <v>55</v>
+      </c>
+      <c r="O15" t="s" s="36">
+        <v>32</v>
+      </c>
+      <c r="P15" t="s" s="45">
+        <v>56</v>
+      </c>
       <c r="Q15" s="38"/>
       <c r="R15" s="36"/>
       <c r="S15" s="39"/>
       <c r="T15" t="s" s="40">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" ht="40.55" customHeight="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" ht="43" customHeight="1">
       <c r="A16" s="30">
         <v>45</v>
       </c>
@@ -2825,29 +2885,37 @@
         <v>27</v>
       </c>
       <c r="D16" t="s" s="31">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s" s="32">
-        <v>51</v>
-      </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
+        <v>58</v>
+      </c>
+      <c r="F16" s="46">
+        <v>44991</v>
+      </c>
+      <c r="G16" t="s" s="35">
+        <v>59</v>
+      </c>
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
-      <c r="J16" s="38"/>
+      <c r="J16" t="s" s="36">
+        <v>32</v>
+      </c>
       <c r="K16" s="37"/>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
-      <c r="N16" s="37"/>
+      <c r="N16" s="43"/>
       <c r="O16" s="38"/>
-      <c r="P16" s="37"/>
+      <c r="P16" t="s" s="42">
+        <v>60</v>
+      </c>
       <c r="Q16" s="38"/>
       <c r="R16" t="s" s="36">
         <v>32</v>
       </c>
       <c r="S16" s="39"/>
       <c r="T16" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" ht="105.55" customHeight="1">
@@ -2861,31 +2929,31 @@
         <v>27</v>
       </c>
       <c r="D17" t="s" s="31">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s" s="32">
-        <v>53</v>
-      </c>
-      <c r="F17" s="33"/>
+        <v>62</v>
+      </c>
+      <c r="F17" s="47"/>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
       <c r="J17" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K17" t="s" s="36">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="L17" s="36"/>
       <c r="M17" s="38"/>
       <c r="N17" s="37"/>
       <c r="O17" s="38"/>
-      <c r="P17" s="37"/>
+      <c r="P17" s="43"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="36"/>
       <c r="S17" s="39"/>
       <c r="T17" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="105.55" customHeight="1">
@@ -2899,10 +2967,10 @@
         <v>27</v>
       </c>
       <c r="D18" t="s" s="31">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s" s="32">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F18" s="33">
         <v>44984</v>
@@ -2911,10 +2979,10 @@
         <v>1677484800</v>
       </c>
       <c r="H18" t="s" s="35">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="I18" t="s" s="35">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J18" t="s" s="36">
         <v>32</v>
@@ -2927,19 +2995,19 @@
         <v>32</v>
       </c>
       <c r="N18" t="s" s="36">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="O18" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P18" t="s" s="36">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="Q18" s="38"/>
       <c r="R18" s="36"/>
       <c r="S18" s="39"/>
       <c r="T18" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" ht="144.55" customHeight="1">
@@ -2953,10 +3021,10 @@
         <v>27</v>
       </c>
       <c r="D19" t="s" s="31">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s" s="32">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F19" s="33">
         <v>44984</v>
@@ -2965,10 +3033,10 @@
         <v>1677485160</v>
       </c>
       <c r="H19" t="s" s="35">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="I19" t="s" s="35">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J19" t="s" s="36">
         <v>32</v>
@@ -2981,19 +3049,19 @@
         <v>32</v>
       </c>
       <c r="N19" t="s" s="36">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="O19" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P19" t="s" s="36">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="Q19" s="38"/>
       <c r="R19" s="36"/>
       <c r="S19" s="39"/>
       <c r="T19" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" ht="131.55" customHeight="1">
@@ -3007,10 +3075,10 @@
         <v>27</v>
       </c>
       <c r="D20" t="s" s="31">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s" s="32">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F20" s="33">
         <v>44984</v>
@@ -3019,10 +3087,10 @@
         <v>1677485340</v>
       </c>
       <c r="H20" t="s" s="35">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s" s="35">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="J20" t="s" s="36">
         <v>32</v>
@@ -3035,19 +3103,19 @@
         <v>32</v>
       </c>
       <c r="N20" t="s" s="36">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="O20" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P20" t="s" s="36">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="Q20" s="38"/>
       <c r="R20" s="36"/>
       <c r="S20" s="39"/>
       <c r="T20" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" ht="118.55" customHeight="1">
@@ -3061,10 +3129,10 @@
         <v>27</v>
       </c>
       <c r="D21" t="s" s="31">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s" s="32">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F21" s="33">
         <v>44984</v>
@@ -3073,10 +3141,10 @@
         <v>1677485520</v>
       </c>
       <c r="H21" t="s" s="35">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s" s="35">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s" s="36">
         <v>32</v>
@@ -3089,19 +3157,19 @@
         <v>32</v>
       </c>
       <c r="N21" t="s" s="36">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="O21" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P21" t="s" s="36">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="Q21" s="38"/>
       <c r="R21" s="36"/>
       <c r="S21" s="39"/>
       <c r="T21" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" ht="105.55" customHeight="1">
@@ -3115,10 +3183,10 @@
         <v>27</v>
       </c>
       <c r="D22" t="s" s="31">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s" s="32">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F22" s="33">
         <v>44984</v>
@@ -3127,10 +3195,10 @@
         <v>1677486000</v>
       </c>
       <c r="H22" t="s" s="35">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I22" t="s" s="35">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="J22" t="s" s="36">
         <v>32</v>
@@ -3143,19 +3211,19 @@
         <v>32</v>
       </c>
       <c r="N22" t="s" s="36">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="O22" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P22" t="s" s="36">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="Q22" s="38"/>
       <c r="R22" s="36"/>
       <c r="S22" s="39"/>
       <c r="T22" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" ht="157.55" customHeight="1">
@@ -3169,10 +3237,10 @@
         <v>27</v>
       </c>
       <c r="D23" t="s" s="31">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s" s="32">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F23" s="33">
         <v>44984</v>
@@ -3181,10 +3249,10 @@
         <v>1677486180</v>
       </c>
       <c r="H23" t="s" s="35">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="I23" t="s" s="35">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="J23" t="s" s="36">
         <v>32</v>
@@ -3197,19 +3265,19 @@
         <v>32</v>
       </c>
       <c r="N23" t="s" s="36">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="O23" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P23" t="s" s="36">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="Q23" s="38"/>
       <c r="R23" s="36"/>
       <c r="S23" s="39"/>
       <c r="T23" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" ht="131.55" customHeight="1">
@@ -3223,10 +3291,10 @@
         <v>27</v>
       </c>
       <c r="D24" t="s" s="31">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s" s="32">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F24" s="33">
         <v>44984</v>
@@ -3235,10 +3303,10 @@
         <v>1677486300</v>
       </c>
       <c r="H24" t="s" s="35">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I24" t="s" s="35">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="J24" t="s" s="36">
         <v>32</v>
@@ -3251,19 +3319,19 @@
         <v>32</v>
       </c>
       <c r="N24" t="s" s="36">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="O24" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P24" t="s" s="36">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="Q24" s="38"/>
       <c r="R24" s="36"/>
       <c r="S24" s="39"/>
       <c r="T24" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" ht="131.55" customHeight="1">
@@ -3277,22 +3345,22 @@
         <v>27</v>
       </c>
       <c r="D25" t="s" s="31">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E25" t="s" s="32">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F25" s="33">
         <v>44984</v>
       </c>
-      <c r="G25" s="42">
+      <c r="G25" s="48">
         <v>1677504360</v>
       </c>
       <c r="H25" t="s" s="35">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="I25" t="s" s="35">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="J25" t="s" s="36">
         <v>32</v>
@@ -3305,19 +3373,19 @@
         <v>32</v>
       </c>
       <c r="N25" t="s" s="36">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="O25" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P25" t="s" s="36">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q25" s="38"/>
       <c r="R25" s="36"/>
       <c r="S25" s="39"/>
       <c r="T25" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" ht="183.55" customHeight="1">
@@ -3331,10 +3399,10 @@
         <v>27</v>
       </c>
       <c r="D26" t="s" s="31">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s" s="32">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F26" s="33">
         <v>44984</v>
@@ -3343,10 +3411,10 @@
         <v>1677504600</v>
       </c>
       <c r="H26" t="s" s="35">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="I26" t="s" s="35">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="J26" t="s" s="36">
         <v>32</v>
@@ -3359,19 +3427,19 @@
         <v>32</v>
       </c>
       <c r="N26" t="s" s="36">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="O26" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="P26" t="s" s="36">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="Q26" s="38"/>
       <c r="R26" s="36"/>
       <c r="S26" s="39"/>
       <c r="T26" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" ht="105.55" customHeight="1">
@@ -3385,20 +3453,20 @@
         <v>27</v>
       </c>
       <c r="D27" t="s" s="31">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s" s="32">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="34"/>
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
       <c r="J27" t="s" s="36">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K27" t="s" s="36">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="L27" s="38"/>
       <c r="M27" s="38"/>
@@ -3409,45 +3477,45 @@
       <c r="R27" s="36"/>
       <c r="S27" s="39"/>
       <c r="T27" t="s" s="40">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" ht="105.05" customHeight="1">
-      <c r="A28" s="43">
+      <c r="A28" s="49">
         <v>74</v>
       </c>
-      <c r="B28" t="s" s="44">
+      <c r="B28" t="s" s="50">
         <v>26</v>
       </c>
-      <c r="C28" t="s" s="44">
+      <c r="C28" t="s" s="50">
         <v>27</v>
       </c>
-      <c r="D28" t="s" s="44">
-        <v>113</v>
-      </c>
-      <c r="E28" t="s" s="45">
-        <v>114</v>
+      <c r="D28" t="s" s="50">
+        <v>121</v>
+      </c>
+      <c r="E28" t="s" s="51">
+        <v>122</v>
       </c>
       <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
+      <c r="G28" s="52"/>
       <c r="H28" s="46"/>
       <c r="I28" s="46"/>
-      <c r="J28" t="s" s="48">
-        <v>54</v>
-      </c>
-      <c r="K28" t="s" s="48">
-        <v>115</v>
-      </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="51"/>
-      <c r="T28" t="s" s="52">
+      <c r="J28" t="s" s="44">
         <v>47</v>
+      </c>
+      <c r="K28" t="s" s="44">
+        <v>123</v>
+      </c>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="55"/>
+      <c r="T28" t="s" s="56">
+        <v>49</v>
       </c>
     </row>
     <row r="29" ht="13.55" customHeight="1">
@@ -3456,21 +3524,21 @@
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="54"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="57"/>
-      <c r="T29" s="54"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="61"/>
+      <c r="T29" s="58"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="3"/>
@@ -22076,123 +22144,123 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="58" customWidth="1"/>
-    <col min="2" max="2" width="23.8516" style="58" customWidth="1"/>
-    <col min="3" max="3" width="18.8516" style="58" customWidth="1"/>
-    <col min="4" max="4" width="58.5" style="58" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="58" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="58" customWidth="1"/>
+    <col min="1" max="1" width="16" style="62" customWidth="1"/>
+    <col min="2" max="2" width="23.8516" style="62" customWidth="1"/>
+    <col min="3" max="3" width="18.8516" style="62" customWidth="1"/>
+    <col min="4" max="4" width="58.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="62" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="59">
+      <c r="A1" t="s" s="63">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="60">
+      <c r="B1" t="s" s="64">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="60">
-        <v>116</v>
-      </c>
-      <c r="D1" t="s" s="61">
-        <v>117</v>
-      </c>
-      <c r="E1" s="62"/>
+      <c r="C1" t="s" s="64">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s" s="65">
+        <v>125</v>
+      </c>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="63">
-        <v>118</v>
-      </c>
-      <c r="B2" t="s" s="64">
-        <v>119</v>
-      </c>
-      <c r="C2" t="s" s="65">
-        <v>120</v>
-      </c>
-      <c r="D2" t="s" s="66">
-        <v>121</v>
-      </c>
-      <c r="E2" s="62"/>
+      <c r="A2" t="s" s="67">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s" s="68">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s" s="69">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s" s="70">
+        <v>129</v>
+      </c>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="67">
+      <c r="A3" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="B3" t="s" s="68">
-        <v>119</v>
-      </c>
-      <c r="C3" t="s" s="69">
-        <v>122</v>
-      </c>
-      <c r="D3" t="s" s="70">
-        <v>123</v>
-      </c>
-      <c r="E3" s="62"/>
+      <c r="B3" t="s" s="72">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s" s="73">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s" s="74">
+        <v>131</v>
+      </c>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="67">
-        <v>124</v>
-      </c>
-      <c r="B4" t="s" s="68">
-        <v>119</v>
-      </c>
-      <c r="C4" t="s" s="69">
-        <v>125</v>
-      </c>
-      <c r="D4" t="s" s="71">
-        <v>126</v>
-      </c>
-      <c r="E4" s="62"/>
+      <c r="A4" t="s" s="71">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s" s="72">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s" s="73">
+        <v>133</v>
+      </c>
+      <c r="D4" t="s" s="75">
+        <v>134</v>
+      </c>
+      <c r="E4" s="66"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="67">
+      <c r="A5" t="s" s="71">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s" s="72">
         <v>127</v>
       </c>
-      <c r="B5" t="s" s="68">
-        <v>119</v>
-      </c>
-      <c r="C5" t="s" s="69">
-        <v>128</v>
-      </c>
-      <c r="D5" t="s" s="70">
-        <v>129</v>
-      </c>
-      <c r="E5" s="62"/>
+      <c r="C5" t="s" s="73">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s" s="74">
+        <v>137</v>
+      </c>
+      <c r="E5" s="66"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="67">
-        <v>130</v>
-      </c>
-      <c r="B6" t="s" s="68">
-        <v>119</v>
-      </c>
-      <c r="C6" t="s" s="69">
-        <v>131</v>
-      </c>
-      <c r="D6" t="s" s="71">
-        <v>132</v>
-      </c>
-      <c r="E6" s="62"/>
+      <c r="A6" t="s" s="71">
+        <v>138</v>
+      </c>
+      <c r="B6" t="s" s="72">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s" s="73">
+        <v>139</v>
+      </c>
+      <c r="D6" t="s" s="75">
+        <v>140</v>
+      </c>
+      <c r="E6" s="66"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" t="s" s="72">
-        <v>133</v>
-      </c>
-      <c r="B7" t="s" s="73">
-        <v>119</v>
-      </c>
-      <c r="C7" t="s" s="74">
-        <v>134</v>
-      </c>
-      <c r="D7" t="s" s="71">
-        <v>135</v>
-      </c>
-      <c r="E7" s="62"/>
+      <c r="A7" t="s" s="76">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s" s="77">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s" s="78">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s" s="75">
+        <v>143</v>
+      </c>
+      <c r="E7" s="66"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="20"/>
       <c r="E8" s="3"/>
     </row>

</xml_diff>

<commit_message>
Corretti errori casi test ID 6,7,8,9
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="145">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -129,10 +129,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>d1983a0e5843491b</t>
+    <t>e045aff956bce175</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.99b8d05aa6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.07719f376c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -149,10 +149,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>e66180cf46503379</t>
+    <t>523c159d780d6fd0</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.f0d4e2ae4b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.5673712add^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -163,10 +163,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>f6b4be07be0a3595</t>
+    <t>a732d13a42cfe45d</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.536ae164ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.e0608032f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -177,7 +177,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.fa01a9d4fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>b1edc3a30d340552</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.2041f6fb1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
@@ -2623,10 +2626,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="33">
-        <v>44986</v>
+        <v>45005</v>
       </c>
       <c r="G10" s="34">
-        <v>1677505200</v>
+        <v>1679299654</v>
       </c>
       <c r="H10" t="s" s="35">
         <v>30</v>
@@ -2667,10 +2670,10 @@
         <v>35</v>
       </c>
       <c r="F11" s="33">
-        <v>44986</v>
+        <v>45005</v>
       </c>
       <c r="G11" s="34">
-        <v>1677668064</v>
+        <v>1679301656</v>
       </c>
       <c r="H11" t="s" s="35">
         <v>36</v>
@@ -2711,10 +2714,10 @@
         <v>39</v>
       </c>
       <c r="F12" s="33">
-        <v>44986</v>
+        <v>45005</v>
       </c>
       <c r="G12" s="34">
-        <v>1677669760</v>
+        <v>1679302308</v>
       </c>
       <c r="H12" t="s" s="35">
         <v>40</v>
@@ -2755,16 +2758,16 @@
         <v>43</v>
       </c>
       <c r="F13" s="33">
-        <v>44986</v>
+        <v>45007</v>
       </c>
       <c r="G13" s="34">
-        <v>1677670068</v>
-      </c>
-      <c r="H13" s="34">
-        <v>6709506444487090</v>
+        <v>1679483150</v>
+      </c>
+      <c r="H13" t="s" s="35">
+        <v>44</v>
       </c>
       <c r="I13" t="s" s="35">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J13" t="s" s="36">
         <v>32</v>
@@ -2793,20 +2796,20 @@
         <v>27</v>
       </c>
       <c r="D14" t="s" s="31">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s" s="41">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
       <c r="J14" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K14" t="s" s="42">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
@@ -2817,7 +2820,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="39"/>
       <c r="T14" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" ht="105.55" customHeight="1">
@@ -2831,22 +2834,22 @@
         <v>27</v>
       </c>
       <c r="D15" t="s" s="31">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s" s="41">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F15" s="33">
         <v>44991</v>
       </c>
       <c r="G15" t="s" s="35">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s" s="35">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" t="s" s="35">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J15" t="s" s="36">
         <v>32</v>
@@ -2856,22 +2859,22 @@
         <v>32</v>
       </c>
       <c r="M15" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N15" t="s" s="44">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O15" t="s" s="36">
         <v>32</v>
       </c>
       <c r="P15" t="s" s="45">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q15" s="38"/>
       <c r="R15" s="36"/>
       <c r="S15" s="39"/>
       <c r="T15" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" ht="43" customHeight="1">
@@ -2885,16 +2888,16 @@
         <v>27</v>
       </c>
       <c r="D16" t="s" s="31">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s" s="32">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16" s="46">
         <v>44991</v>
       </c>
       <c r="G16" t="s" s="35">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
@@ -2907,7 +2910,7 @@
       <c r="N16" s="43"/>
       <c r="O16" s="38"/>
       <c r="P16" t="s" s="42">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q16" s="38"/>
       <c r="R16" t="s" s="36">
@@ -2915,7 +2918,7 @@
       </c>
       <c r="S16" s="39"/>
       <c r="T16" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" ht="105.55" customHeight="1">
@@ -2929,20 +2932,20 @@
         <v>27</v>
       </c>
       <c r="D17" t="s" s="31">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s" s="32">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" s="47"/>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
       <c r="J17" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K17" t="s" s="36">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L17" s="36"/>
       <c r="M17" s="38"/>
@@ -2953,7 +2956,7 @@
       <c r="R17" s="36"/>
       <c r="S17" s="39"/>
       <c r="T17" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="105.55" customHeight="1">
@@ -2967,10 +2970,10 @@
         <v>27</v>
       </c>
       <c r="D18" t="s" s="31">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s" s="32">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F18" s="33">
         <v>44984</v>
@@ -2979,10 +2982,10 @@
         <v>1677484800</v>
       </c>
       <c r="H18" t="s" s="35">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s" s="35">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J18" t="s" s="36">
         <v>32</v>
@@ -2995,19 +2998,19 @@
         <v>32</v>
       </c>
       <c r="N18" t="s" s="36">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O18" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P18" t="s" s="36">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q18" s="38"/>
       <c r="R18" s="36"/>
       <c r="S18" s="39"/>
       <c r="T18" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" ht="144.55" customHeight="1">
@@ -3021,10 +3024,10 @@
         <v>27</v>
       </c>
       <c r="D19" t="s" s="31">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s" s="32">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F19" s="33">
         <v>44984</v>
@@ -3033,10 +3036,10 @@
         <v>1677485160</v>
       </c>
       <c r="H19" t="s" s="35">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s" s="35">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J19" t="s" s="36">
         <v>32</v>
@@ -3049,19 +3052,19 @@
         <v>32</v>
       </c>
       <c r="N19" t="s" s="36">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O19" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P19" t="s" s="36">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q19" s="38"/>
       <c r="R19" s="36"/>
       <c r="S19" s="39"/>
       <c r="T19" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" ht="131.55" customHeight="1">
@@ -3075,10 +3078,10 @@
         <v>27</v>
       </c>
       <c r="D20" t="s" s="31">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s" s="32">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F20" s="33">
         <v>44984</v>
@@ -3087,10 +3090,10 @@
         <v>1677485340</v>
       </c>
       <c r="H20" t="s" s="35">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I20" t="s" s="35">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J20" t="s" s="36">
         <v>32</v>
@@ -3103,19 +3106,19 @@
         <v>32</v>
       </c>
       <c r="N20" t="s" s="36">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O20" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P20" t="s" s="36">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="38"/>
       <c r="R20" s="36"/>
       <c r="S20" s="39"/>
       <c r="T20" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" ht="118.55" customHeight="1">
@@ -3129,10 +3132,10 @@
         <v>27</v>
       </c>
       <c r="D21" t="s" s="31">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s" s="32">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F21" s="33">
         <v>44984</v>
@@ -3141,10 +3144,10 @@
         <v>1677485520</v>
       </c>
       <c r="H21" t="s" s="35">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I21" t="s" s="35">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J21" t="s" s="36">
         <v>32</v>
@@ -3157,19 +3160,19 @@
         <v>32</v>
       </c>
       <c r="N21" t="s" s="36">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O21" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P21" t="s" s="36">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Q21" s="38"/>
       <c r="R21" s="36"/>
       <c r="S21" s="39"/>
       <c r="T21" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" ht="105.55" customHeight="1">
@@ -3183,10 +3186,10 @@
         <v>27</v>
       </c>
       <c r="D22" t="s" s="31">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s" s="32">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F22" s="33">
         <v>44984</v>
@@ -3195,10 +3198,10 @@
         <v>1677486000</v>
       </c>
       <c r="H22" t="s" s="35">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I22" t="s" s="35">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J22" t="s" s="36">
         <v>32</v>
@@ -3211,19 +3214,19 @@
         <v>32</v>
       </c>
       <c r="N22" t="s" s="36">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O22" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P22" t="s" s="36">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q22" s="38"/>
       <c r="R22" s="36"/>
       <c r="S22" s="39"/>
       <c r="T22" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" ht="157.55" customHeight="1">
@@ -3237,10 +3240,10 @@
         <v>27</v>
       </c>
       <c r="D23" t="s" s="31">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s" s="32">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F23" s="33">
         <v>44984</v>
@@ -3249,10 +3252,10 @@
         <v>1677486180</v>
       </c>
       <c r="H23" t="s" s="35">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I23" t="s" s="35">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J23" t="s" s="36">
         <v>32</v>
@@ -3265,19 +3268,19 @@
         <v>32</v>
       </c>
       <c r="N23" t="s" s="36">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O23" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P23" t="s" s="36">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Q23" s="38"/>
       <c r="R23" s="36"/>
       <c r="S23" s="39"/>
       <c r="T23" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" ht="131.55" customHeight="1">
@@ -3291,10 +3294,10 @@
         <v>27</v>
       </c>
       <c r="D24" t="s" s="31">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s" s="32">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F24" s="33">
         <v>44984</v>
@@ -3303,10 +3306,10 @@
         <v>1677486300</v>
       </c>
       <c r="H24" t="s" s="35">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I24" t="s" s="35">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J24" t="s" s="36">
         <v>32</v>
@@ -3319,19 +3322,19 @@
         <v>32</v>
       </c>
       <c r="N24" t="s" s="36">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O24" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P24" t="s" s="36">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q24" s="38"/>
       <c r="R24" s="36"/>
       <c r="S24" s="39"/>
       <c r="T24" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" ht="131.55" customHeight="1">
@@ -3345,10 +3348,10 @@
         <v>27</v>
       </c>
       <c r="D25" t="s" s="31">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s" s="32">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F25" s="33">
         <v>44984</v>
@@ -3357,10 +3360,10 @@
         <v>1677504360</v>
       </c>
       <c r="H25" t="s" s="35">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I25" t="s" s="35">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J25" t="s" s="36">
         <v>32</v>
@@ -3373,19 +3376,19 @@
         <v>32</v>
       </c>
       <c r="N25" t="s" s="36">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O25" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P25" t="s" s="36">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q25" s="38"/>
       <c r="R25" s="36"/>
       <c r="S25" s="39"/>
       <c r="T25" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" ht="183.55" customHeight="1">
@@ -3399,10 +3402,10 @@
         <v>27</v>
       </c>
       <c r="D26" t="s" s="31">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s" s="32">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F26" s="33">
         <v>44984</v>
@@ -3411,10 +3414,10 @@
         <v>1677504600</v>
       </c>
       <c r="H26" t="s" s="35">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s" s="35">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J26" t="s" s="36">
         <v>32</v>
@@ -3427,19 +3430,19 @@
         <v>32</v>
       </c>
       <c r="N26" t="s" s="36">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O26" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P26" t="s" s="36">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q26" s="38"/>
       <c r="R26" s="36"/>
       <c r="S26" s="39"/>
       <c r="T26" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" ht="105.55" customHeight="1">
@@ -3453,20 +3456,20 @@
         <v>27</v>
       </c>
       <c r="D27" t="s" s="31">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E27" t="s" s="32">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="34"/>
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
       <c r="J27" t="s" s="36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K27" t="s" s="36">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L27" s="38"/>
       <c r="M27" s="38"/>
@@ -3477,7 +3480,7 @@
       <c r="R27" s="36"/>
       <c r="S27" s="39"/>
       <c r="T27" t="s" s="40">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" ht="105.05" customHeight="1">
@@ -3491,20 +3494,20 @@
         <v>27</v>
       </c>
       <c r="D28" t="s" s="50">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E28" t="s" s="51">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F28" s="46"/>
       <c r="G28" s="52"/>
       <c r="H28" s="46"/>
       <c r="I28" s="46"/>
       <c r="J28" t="s" s="44">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K28" t="s" s="44">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L28" s="53"/>
       <c r="M28" s="53"/>
@@ -3515,7 +3518,7 @@
       <c r="R28" s="44"/>
       <c r="S28" s="55"/>
       <c r="T28" t="s" s="56">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" ht="13.55" customHeight="1">
@@ -22160,25 +22163,25 @@
         <v>7</v>
       </c>
       <c r="C1" t="s" s="64">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s" s="65">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E1" s="66"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="67">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="68">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s" s="69">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s" s="70">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E2" s="66"/>
     </row>
@@ -22187,73 +22190,73 @@
         <v>27</v>
       </c>
       <c r="B3" t="s" s="72">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s" s="73">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s" s="74">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E3" s="66"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="71">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s" s="72">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s" s="73">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s" s="75">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E4" s="66"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s" s="71">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s" s="72">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s" s="73">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s" s="74">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E5" s="66"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s" s="71">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s" s="72">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s" s="73">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s" s="75">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E6" s="66"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s" s="76">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s" s="77">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s" s="78">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s" s="75">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E7" s="66"/>
     </row>

</xml_diff>

<commit_message>
Corretti errori; aggiornato data.json; aggiornato report
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
@@ -52,7 +52,7 @@
     <t>subject_application_vendor: GESAN SRL</t>
   </si>
   <si>
-    <t>subject_application_version: v.2.0</t>
+    <t>subject_application_version: V.2.0</t>
   </si>
   <si>
     <t>ID</t>
@@ -129,10 +129,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>e045aff956bce175</t>
+    <t>63de9e29674fcffb</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.07719f376c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.f5cf37717d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -149,10 +149,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>523c159d780d6fd0</t>
+    <t>4037fec3c4107ef7</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.5673712add^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.df710ec06f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -163,10 +163,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>a732d13a42cfe45d</t>
+    <t>ece81a3b0b395717</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.e0608032f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.5dfa4514e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -177,10 +177,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>b1edc3a30d340552</t>
+    <t>e2d5bdec1391802c</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.2041f6fb1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.b810e36e1d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
@@ -303,13 +303,13 @@
     </r>
   </si>
   <si>
-    <t>11:01:00</t>
+    <t>11:59:00</t>
   </si>
   <si>
-    <t>8c463e33a4928d82</t>
+    <t>bb69426c3015b737</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.44cc2c90f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.0689d1ea86^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>JWT payload: Tipologia documento diversa dalla tipologia di CDA (code - codesystem)</t>
@@ -350,10 +350,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>9e70c80ad9e2834d</t>
+    <t>7897782f5b2d57ca</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.99a3640ff4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.8429adb4c2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico.[Errore-47| codice fiscale '' cittadino ed operatore: 16 cifre [A-Z0-9]{16}],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -370,10 +370,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>451dc4b5696825ad</t>
+    <t>9c8de420b83b5b38</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.14b3e28240^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.52f68861f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico. [ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -390,10 +390,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>23f693872bf8be6f</t>
+    <t>0c1e6069535dc67a</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.653797668f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.d193dd6fbe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico . [ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -410,10 +410,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>670cf5fbec5f79cc</t>
+    <t>9fef5168f21020f7</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.89c750aa48^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.29d87765c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico. [ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -430,10 +430,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>3512e09548c4c873</t>
+    <t>7a1ffe9aac03863f</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.fb39283d8f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.bd6064c0d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore vocabolario. Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: G]</t>
@@ -450,10 +450,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>1fb6ab7d866af2b4</t>
+    <t>e4f3cbc20889c3e2</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.b18d4a1e3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.91d22d0c4f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico. [ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -471,10 +471,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>3b5d98bb72e2a2f0</t>
+    <t>1583b241a9c647b2</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.ca8ff9dcb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.17a9c8936d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico. [ERRORE-b3| Sezione Decorso Ospedaliero: la sezione DEVE essere presente],[ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
@@ -492,10 +492,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>e2f04779b31c4990</t>
+    <t>d3f67b8a79e444eb</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.37a211a4f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.97c62839c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico. [W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ],[ERRORE-b26| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]</t>
@@ -512,10 +512,10 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>61b7330185409ce1</t>
+    <t>a8e976281f1edd33</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.e83c307003^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.35a5b3ae06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico. [W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ],[ERRORE-b25| Sotto-sezione Anamnesi: l'elemento entry/observation/statusCode deve avere l'attributo @code='completed'],[ERRORE-b26| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]</t>
@@ -992,7 +992,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1095,7 +1095,7 @@
     <xf numFmtId="59" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1116,8 +1116,20 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1131,13 +1143,10 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="21" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2626,10 +2635,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="33">
-        <v>45005</v>
+        <v>45013</v>
       </c>
       <c r="G10" s="34">
-        <v>1679299654</v>
+        <v>45013.489583333336</v>
       </c>
       <c r="H10" t="s" s="35">
         <v>30</v>
@@ -2670,10 +2679,10 @@
         <v>35</v>
       </c>
       <c r="F11" s="33">
-        <v>45005</v>
+        <v>45013</v>
       </c>
       <c r="G11" s="34">
-        <v>1679301656</v>
+        <v>45013.490277777775</v>
       </c>
       <c r="H11" t="s" s="35">
         <v>36</v>
@@ -2714,10 +2723,10 @@
         <v>39</v>
       </c>
       <c r="F12" s="33">
-        <v>45005</v>
+        <v>45013</v>
       </c>
       <c r="G12" s="34">
-        <v>1679302308</v>
+        <v>45013.490972222222</v>
       </c>
       <c r="H12" t="s" s="35">
         <v>40</v>
@@ -2757,16 +2766,16 @@
       <c r="E13" t="s" s="32">
         <v>43</v>
       </c>
-      <c r="F13" s="33">
-        <v>45007</v>
-      </c>
-      <c r="G13" s="34">
-        <v>1679483150</v>
-      </c>
-      <c r="H13" t="s" s="35">
+      <c r="F13" s="41">
+        <v>45013</v>
+      </c>
+      <c r="G13" s="42">
+        <v>45013.491666666669</v>
+      </c>
+      <c r="H13" t="s" s="43">
         <v>44</v>
       </c>
-      <c r="I13" t="s" s="35">
+      <c r="I13" t="s" s="43">
         <v>45</v>
       </c>
       <c r="J13" t="s" s="36">
@@ -2798,17 +2807,17 @@
       <c r="D14" t="s" s="31">
         <v>46</v>
       </c>
-      <c r="E14" t="s" s="41">
+      <c r="E14" t="s" s="44">
         <v>47</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
       <c r="J14" t="s" s="36">
         <v>48</v>
       </c>
-      <c r="K14" t="s" s="42">
+      <c r="K14" t="s" s="46">
         <v>49</v>
       </c>
       <c r="L14" s="38"/>
@@ -2836,38 +2845,38 @@
       <c r="D15" t="s" s="31">
         <v>51</v>
       </c>
-      <c r="E15" t="s" s="41">
+      <c r="E15" t="s" s="44">
         <v>52</v>
       </c>
       <c r="F15" s="33">
-        <v>44991</v>
+        <v>45013</v>
       </c>
       <c r="G15" t="s" s="35">
         <v>53</v>
       </c>
-      <c r="H15" t="s" s="35">
+      <c r="H15" t="s" s="43">
         <v>54</v>
       </c>
-      <c r="I15" t="s" s="35">
+      <c r="I15" t="s" s="43">
         <v>55</v>
       </c>
       <c r="J15" t="s" s="36">
         <v>32</v>
       </c>
-      <c r="K15" s="43"/>
+      <c r="K15" s="47"/>
       <c r="L15" t="s" s="36">
         <v>32</v>
       </c>
       <c r="M15" t="s" s="36">
         <v>48</v>
       </c>
-      <c r="N15" t="s" s="44">
+      <c r="N15" t="s" s="48">
         <v>56</v>
       </c>
       <c r="O15" t="s" s="36">
         <v>32</v>
       </c>
-      <c r="P15" t="s" s="45">
+      <c r="P15" t="s" s="49">
         <v>57</v>
       </c>
       <c r="Q15" s="38"/>
@@ -2893,23 +2902,23 @@
       <c r="E16" t="s" s="32">
         <v>59</v>
       </c>
-      <c r="F16" s="46">
+      <c r="F16" s="41">
         <v>44991</v>
       </c>
       <c r="G16" t="s" s="35">
         <v>60</v>
       </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
       <c r="J16" t="s" s="36">
         <v>32</v>
       </c>
       <c r="K16" s="37"/>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
-      <c r="N16" s="43"/>
+      <c r="N16" s="47"/>
       <c r="O16" s="38"/>
-      <c r="P16" t="s" s="42">
+      <c r="P16" t="s" s="46">
         <v>61</v>
       </c>
       <c r="Q16" s="38"/>
@@ -2937,7 +2946,7 @@
       <c r="E17" t="s" s="32">
         <v>63</v>
       </c>
-      <c r="F17" s="47"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
@@ -2951,7 +2960,7 @@
       <c r="M17" s="38"/>
       <c r="N17" s="37"/>
       <c r="O17" s="38"/>
-      <c r="P17" s="43"/>
+      <c r="P17" s="47"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="36"/>
       <c r="S17" s="39"/>
@@ -2976,10 +2985,10 @@
         <v>66</v>
       </c>
       <c r="F18" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G18" s="34">
-        <v>1677484800</v>
+        <v>45013.49375</v>
       </c>
       <c r="H18" t="s" s="35">
         <v>67</v>
@@ -3030,10 +3039,10 @@
         <v>72</v>
       </c>
       <c r="F19" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G19" s="34">
-        <v>1677485160</v>
+        <v>45013.495138888888</v>
       </c>
       <c r="H19" t="s" s="35">
         <v>73</v>
@@ -3084,10 +3093,10 @@
         <v>78</v>
       </c>
       <c r="F20" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G20" s="34">
-        <v>1677485340</v>
+        <v>45013.495833333334</v>
       </c>
       <c r="H20" t="s" s="35">
         <v>79</v>
@@ -3138,10 +3147,10 @@
         <v>84</v>
       </c>
       <c r="F21" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G21" s="34">
-        <v>1677485520</v>
+        <v>45013.495833333334</v>
       </c>
       <c r="H21" t="s" s="35">
         <v>85</v>
@@ -3192,10 +3201,10 @@
         <v>90</v>
       </c>
       <c r="F22" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G22" s="34">
-        <v>1677486000</v>
+        <v>45013.496527777781</v>
       </c>
       <c r="H22" t="s" s="35">
         <v>91</v>
@@ -3246,10 +3255,10 @@
         <v>96</v>
       </c>
       <c r="F23" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G23" s="34">
-        <v>1677486180</v>
+        <v>45013.497222222220</v>
       </c>
       <c r="H23" t="s" s="35">
         <v>97</v>
@@ -3300,10 +3309,10 @@
         <v>102</v>
       </c>
       <c r="F24" s="33">
-        <v>44984</v>
+        <v>45013</v>
       </c>
       <c r="G24" s="34">
-        <v>1677486300</v>
+        <v>45013.497222222220</v>
       </c>
       <c r="H24" t="s" s="35">
         <v>103</v>
@@ -3354,10 +3363,10 @@
         <v>108</v>
       </c>
       <c r="F25" s="33">
-        <v>44984</v>
-      </c>
-      <c r="G25" s="48">
-        <v>1677504360</v>
+        <v>45013</v>
+      </c>
+      <c r="G25" s="50">
+        <v>45013.497916666667</v>
       </c>
       <c r="H25" t="s" s="35">
         <v>109</v>
@@ -3407,16 +3416,16 @@
       <c r="E26" t="s" s="32">
         <v>114</v>
       </c>
-      <c r="F26" s="33">
-        <v>44984</v>
+      <c r="F26" s="41">
+        <v>45013</v>
       </c>
       <c r="G26" s="34">
-        <v>1677504600</v>
-      </c>
-      <c r="H26" t="s" s="35">
+        <v>45013.498611111114</v>
+      </c>
+      <c r="H26" t="s" s="43">
         <v>115</v>
       </c>
-      <c r="I26" t="s" s="35">
+      <c r="I26" t="s" s="43">
         <v>116</v>
       </c>
       <c r="J26" t="s" s="36">
@@ -3461,10 +3470,10 @@
       <c r="E27" t="s" s="32">
         <v>120</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
       <c r="J27" t="s" s="36">
         <v>48</v>
       </c>
@@ -3484,40 +3493,40 @@
       </c>
     </row>
     <row r="28" ht="105.05" customHeight="1">
-      <c r="A28" s="49">
+      <c r="A28" s="52">
         <v>74</v>
       </c>
-      <c r="B28" t="s" s="50">
+      <c r="B28" t="s" s="53">
         <v>26</v>
       </c>
-      <c r="C28" t="s" s="50">
+      <c r="C28" t="s" s="53">
         <v>27</v>
       </c>
-      <c r="D28" t="s" s="50">
+      <c r="D28" t="s" s="53">
         <v>122</v>
       </c>
-      <c r="E28" t="s" s="51">
+      <c r="E28" t="s" s="54">
         <v>123</v>
       </c>
-      <c r="F28" s="46"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
-      <c r="J28" t="s" s="44">
+      <c r="F28" s="41"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" t="s" s="48">
         <v>48</v>
       </c>
-      <c r="K28" t="s" s="44">
+      <c r="K28" t="s" s="48">
         <v>124</v>
       </c>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="54"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="55"/>
-      <c r="T28" t="s" s="56">
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="58"/>
+      <c r="T28" t="s" s="59">
         <v>50</v>
       </c>
     </row>
@@ -3527,21 +3536,21 @@
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="58"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="58"/>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="60"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="58"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="62"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="61"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="3"/>
@@ -22147,123 +22156,123 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="62" customWidth="1"/>
-    <col min="2" max="2" width="23.8516" style="62" customWidth="1"/>
-    <col min="3" max="3" width="18.8516" style="62" customWidth="1"/>
-    <col min="4" max="4" width="58.5" style="62" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="62" customWidth="1"/>
+    <col min="1" max="1" width="16" style="65" customWidth="1"/>
+    <col min="2" max="2" width="23.8516" style="65" customWidth="1"/>
+    <col min="3" max="3" width="18.8516" style="65" customWidth="1"/>
+    <col min="4" max="4" width="58.5" style="65" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="65" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="63">
+      <c r="A1" t="s" s="66">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="64">
+      <c r="B1" t="s" s="67">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="64">
+      <c r="C1" t="s" s="67">
         <v>125</v>
       </c>
-      <c r="D1" t="s" s="65">
+      <c r="D1" t="s" s="68">
         <v>126</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="67">
+      <c r="A2" t="s" s="70">
         <v>127</v>
       </c>
-      <c r="B2" t="s" s="68">
+      <c r="B2" t="s" s="71">
         <v>128</v>
       </c>
-      <c r="C2" t="s" s="69">
+      <c r="C2" t="s" s="72">
         <v>129</v>
       </c>
-      <c r="D2" t="s" s="70">
+      <c r="D2" t="s" s="73">
         <v>130</v>
       </c>
-      <c r="E2" s="66"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="71">
+      <c r="A3" t="s" s="74">
         <v>27</v>
       </c>
-      <c r="B3" t="s" s="72">
+      <c r="B3" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C3" t="s" s="73">
+      <c r="C3" t="s" s="76">
         <v>131</v>
       </c>
-      <c r="D3" t="s" s="74">
+      <c r="D3" t="s" s="77">
         <v>132</v>
       </c>
-      <c r="E3" s="66"/>
+      <c r="E3" s="69"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="71">
+      <c r="A4" t="s" s="74">
         <v>133</v>
       </c>
-      <c r="B4" t="s" s="72">
+      <c r="B4" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C4" t="s" s="73">
+      <c r="C4" t="s" s="76">
         <v>134</v>
       </c>
-      <c r="D4" t="s" s="75">
+      <c r="D4" t="s" s="78">
         <v>135</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="69"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="71">
+      <c r="A5" t="s" s="74">
         <v>136</v>
       </c>
-      <c r="B5" t="s" s="72">
+      <c r="B5" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C5" t="s" s="73">
+      <c r="C5" t="s" s="76">
         <v>137</v>
       </c>
-      <c r="D5" t="s" s="74">
+      <c r="D5" t="s" s="77">
         <v>138</v>
       </c>
-      <c r="E5" s="66"/>
+      <c r="E5" s="69"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="71">
+      <c r="A6" t="s" s="74">
         <v>139</v>
       </c>
-      <c r="B6" t="s" s="72">
+      <c r="B6" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C6" t="s" s="73">
+      <c r="C6" t="s" s="76">
         <v>140</v>
       </c>
-      <c r="D6" t="s" s="75">
+      <c r="D6" t="s" s="78">
         <v>141</v>
       </c>
-      <c r="E6" s="66"/>
+      <c r="E6" s="69"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" t="s" s="76">
+      <c r="A7" t="s" s="79">
         <v>142</v>
       </c>
-      <c r="B7" t="s" s="77">
+      <c r="B7" t="s" s="80">
         <v>128</v>
       </c>
-      <c r="C7" t="s" s="78">
+      <c r="C7" t="s" s="81">
         <v>143</v>
       </c>
-      <c r="D7" t="s" s="75">
+      <c r="D7" t="s" s="78">
         <v>144</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="69"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="20"/>
       <c r="E8" s="3"/>
     </row>

</xml_diff>

<commit_message>
Corretti errori casi test  ID 7, 8, 9
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
@@ -149,10 +149,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>d06de30760be9db9</t>
+    <t>9901929bf6973b8e</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.a56c90b51a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.23aa9a5573^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -163,10 +163,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>6e6b2c2feffdb219</t>
+    <t>306967711b387a4f</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.456cea59c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.1c315e9227^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -177,10 +177,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>c23fe795b89460d8</t>
+    <t>46b719a207b578f5</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.2e7d61172b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.eb862203ed^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
@@ -2676,10 +2676,10 @@
         <v>35</v>
       </c>
       <c r="F11" s="33">
-        <v>45014</v>
+        <v>45028</v>
       </c>
       <c r="G11" s="34">
-        <v>1680078995</v>
+        <v>1681304640</v>
       </c>
       <c r="H11" t="s" s="35">
         <v>36</v>
@@ -2720,10 +2720,10 @@
         <v>39</v>
       </c>
       <c r="F12" s="33">
-        <v>45014</v>
+        <v>45028</v>
       </c>
       <c r="G12" s="34">
-        <v>1680079558</v>
+        <v>1681304842</v>
       </c>
       <c r="H12" t="s" s="35">
         <v>40</v>
@@ -2764,10 +2764,10 @@
         <v>43</v>
       </c>
       <c r="F13" s="41">
-        <v>45014</v>
+        <v>45028</v>
       </c>
       <c r="G13" s="42">
-        <v>1680081362</v>
+        <v>1681304942</v>
       </c>
       <c r="H13" t="s" s="43">
         <v>44</v>

</xml_diff>

<commit_message>
Risolti errori validatore offline
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LDO/v.2.0/report-checklist.xlsx
@@ -177,10 +177,10 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>46b719a207b578f5</t>
+    <t>2378fe2e98cebb0e</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.eb862203ed^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.ac31791c050ccc1bddbbe25b46d3b88bfef981b9d62153a7ab40b3f1f4a6eef5.d43c8e4a0a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
@@ -615,7 +615,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -645,6 +645,11 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Menlo Regular"/>
     </font>
     <font>
       <u val="single"/>
@@ -992,7 +997,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1122,16 +1127,19 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1140,13 +1148,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="21" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="21" fontId="8" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2851,29 +2859,29 @@
       <c r="G15" t="s" s="35">
         <v>53</v>
       </c>
-      <c r="H15" t="s" s="43">
+      <c r="H15" t="s" s="47">
         <v>54</v>
       </c>
-      <c r="I15" t="s" s="43">
+      <c r="I15" t="s" s="47">
         <v>55</v>
       </c>
       <c r="J15" t="s" s="36">
         <v>32</v>
       </c>
-      <c r="K15" s="47"/>
+      <c r="K15" s="48"/>
       <c r="L15" t="s" s="36">
         <v>32</v>
       </c>
       <c r="M15" t="s" s="36">
         <v>48</v>
       </c>
-      <c r="N15" t="s" s="48">
+      <c r="N15" t="s" s="49">
         <v>56</v>
       </c>
       <c r="O15" t="s" s="36">
         <v>32</v>
       </c>
-      <c r="P15" t="s" s="49">
+      <c r="P15" t="s" s="50">
         <v>57</v>
       </c>
       <c r="Q15" s="38"/>
@@ -2913,7 +2921,7 @@
       <c r="K16" s="37"/>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
-      <c r="N16" s="47"/>
+      <c r="N16" s="48"/>
       <c r="O16" s="38"/>
       <c r="P16" t="s" s="46">
         <v>61</v>
@@ -2957,7 +2965,7 @@
       <c r="M17" s="38"/>
       <c r="N17" s="37"/>
       <c r="O17" s="38"/>
-      <c r="P17" s="47"/>
+      <c r="P17" s="48"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="36"/>
       <c r="S17" s="39"/>
@@ -2984,7 +2992,7 @@
       <c r="F18" s="33">
         <v>45013</v>
       </c>
-      <c r="G18" s="50">
+      <c r="G18" s="51">
         <v>45013.49375</v>
       </c>
       <c r="H18" t="s" s="35">
@@ -3038,7 +3046,7 @@
       <c r="F19" s="33">
         <v>45013</v>
       </c>
-      <c r="G19" s="50">
+      <c r="G19" s="51">
         <v>45013.495138888888</v>
       </c>
       <c r="H19" t="s" s="35">
@@ -3092,7 +3100,7 @@
       <c r="F20" s="33">
         <v>45013</v>
       </c>
-      <c r="G20" s="50">
+      <c r="G20" s="51">
         <v>45013.495833333334</v>
       </c>
       <c r="H20" t="s" s="35">
@@ -3146,7 +3154,7 @@
       <c r="F21" s="33">
         <v>45013</v>
       </c>
-      <c r="G21" s="50">
+      <c r="G21" s="51">
         <v>45013.495833333334</v>
       </c>
       <c r="H21" t="s" s="35">
@@ -3200,7 +3208,7 @@
       <c r="F22" s="33">
         <v>45013</v>
       </c>
-      <c r="G22" s="50">
+      <c r="G22" s="51">
         <v>45013.496527777781</v>
       </c>
       <c r="H22" t="s" s="35">
@@ -3254,7 +3262,7 @@
       <c r="F23" s="33">
         <v>45013</v>
       </c>
-      <c r="G23" s="50">
+      <c r="G23" s="51">
         <v>45013.497222222220</v>
       </c>
       <c r="H23" t="s" s="35">
@@ -3308,7 +3316,7 @@
       <c r="F24" s="33">
         <v>45013</v>
       </c>
-      <c r="G24" s="50">
+      <c r="G24" s="51">
         <v>45013.497222222220</v>
       </c>
       <c r="H24" t="s" s="35">
@@ -3362,7 +3370,7 @@
       <c r="F25" s="33">
         <v>45013</v>
       </c>
-      <c r="G25" s="51">
+      <c r="G25" s="52">
         <v>45013.497916666667</v>
       </c>
       <c r="H25" t="s" s="35">
@@ -3416,13 +3424,13 @@
       <c r="F26" s="41">
         <v>45013</v>
       </c>
-      <c r="G26" s="50">
+      <c r="G26" s="51">
         <v>45013.498611111114</v>
       </c>
-      <c r="H26" t="s" s="43">
+      <c r="H26" t="s" s="47">
         <v>115</v>
       </c>
-      <c r="I26" t="s" s="43">
+      <c r="I26" t="s" s="47">
         <v>116</v>
       </c>
       <c r="J26" t="s" s="36">
@@ -3490,40 +3498,40 @@
       </c>
     </row>
     <row r="28" ht="313.05" customHeight="1">
-      <c r="A28" s="52">
+      <c r="A28" s="53">
         <v>74</v>
       </c>
-      <c r="B28" t="s" s="53">
+      <c r="B28" t="s" s="54">
         <v>26</v>
       </c>
-      <c r="C28" t="s" s="53">
+      <c r="C28" t="s" s="54">
         <v>27</v>
       </c>
-      <c r="D28" t="s" s="53">
+      <c r="D28" t="s" s="54">
         <v>122</v>
       </c>
-      <c r="E28" t="s" s="54">
+      <c r="E28" t="s" s="55">
         <v>123</v>
       </c>
       <c r="F28" s="41"/>
       <c r="G28" s="42"/>
       <c r="H28" s="41"/>
       <c r="I28" s="41"/>
-      <c r="J28" t="s" s="48">
+      <c r="J28" t="s" s="49">
         <v>48</v>
       </c>
-      <c r="K28" t="s" s="48">
+      <c r="K28" t="s" s="49">
         <v>124</v>
       </c>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="57"/>
-      <c r="T28" t="s" s="58">
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="58"/>
+      <c r="T28" t="s" s="59">
         <v>50</v>
       </c>
     </row>
@@ -3533,21 +3541,21 @@
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="61"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="62"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="62"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="61"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="3"/>
@@ -22153,123 +22161,123 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="64" customWidth="1"/>
-    <col min="2" max="2" width="23.8516" style="64" customWidth="1"/>
-    <col min="3" max="3" width="18.8516" style="64" customWidth="1"/>
-    <col min="4" max="4" width="58.5" style="64" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="64" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="64" customWidth="1"/>
+    <col min="1" max="1" width="16" style="65" customWidth="1"/>
+    <col min="2" max="2" width="23.8516" style="65" customWidth="1"/>
+    <col min="3" max="3" width="18.8516" style="65" customWidth="1"/>
+    <col min="4" max="4" width="58.5" style="65" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="65" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="65">
+      <c r="A1" t="s" s="66">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="66">
+      <c r="B1" t="s" s="67">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="66">
+      <c r="C1" t="s" s="67">
         <v>125</v>
       </c>
-      <c r="D1" t="s" s="67">
+      <c r="D1" t="s" s="68">
         <v>126</v>
       </c>
-      <c r="E1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="69">
+      <c r="A2" t="s" s="70">
         <v>127</v>
       </c>
-      <c r="B2" t="s" s="70">
+      <c r="B2" t="s" s="71">
         <v>128</v>
       </c>
-      <c r="C2" t="s" s="71">
+      <c r="C2" t="s" s="72">
         <v>129</v>
       </c>
-      <c r="D2" t="s" s="72">
+      <c r="D2" t="s" s="73">
         <v>130</v>
       </c>
-      <c r="E2" s="68"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="73">
+      <c r="A3" t="s" s="74">
         <v>27</v>
       </c>
-      <c r="B3" t="s" s="74">
+      <c r="B3" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C3" t="s" s="75">
+      <c r="C3" t="s" s="76">
         <v>131</v>
       </c>
-      <c r="D3" t="s" s="76">
+      <c r="D3" t="s" s="77">
         <v>132</v>
       </c>
-      <c r="E3" s="68"/>
+      <c r="E3" s="69"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="73">
+      <c r="A4" t="s" s="74">
         <v>133</v>
       </c>
-      <c r="B4" t="s" s="74">
+      <c r="B4" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C4" t="s" s="75">
+      <c r="C4" t="s" s="76">
         <v>134</v>
       </c>
-      <c r="D4" t="s" s="77">
+      <c r="D4" t="s" s="78">
         <v>135</v>
       </c>
-      <c r="E4" s="68"/>
+      <c r="E4" s="69"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="73">
+      <c r="A5" t="s" s="74">
         <v>136</v>
       </c>
-      <c r="B5" t="s" s="74">
+      <c r="B5" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C5" t="s" s="75">
+      <c r="C5" t="s" s="76">
         <v>137</v>
       </c>
-      <c r="D5" t="s" s="76">
+      <c r="D5" t="s" s="77">
         <v>138</v>
       </c>
-      <c r="E5" s="68"/>
+      <c r="E5" s="69"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="73">
+      <c r="A6" t="s" s="74">
         <v>139</v>
       </c>
-      <c r="B6" t="s" s="74">
+      <c r="B6" t="s" s="75">
         <v>128</v>
       </c>
-      <c r="C6" t="s" s="75">
+      <c r="C6" t="s" s="76">
         <v>140</v>
       </c>
-      <c r="D6" t="s" s="77">
+      <c r="D6" t="s" s="78">
         <v>141</v>
       </c>
-      <c r="E6" s="68"/>
+      <c r="E6" s="69"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" t="s" s="78">
+      <c r="A7" t="s" s="79">
         <v>142</v>
       </c>
-      <c r="B7" t="s" s="79">
+      <c r="B7" t="s" s="80">
         <v>128</v>
       </c>
-      <c r="C7" t="s" s="80">
+      <c r="C7" t="s" s="81">
         <v>143</v>
       </c>
-      <c r="D7" t="s" s="77">
+      <c r="D7" t="s" s="78">
         <v>144</v>
       </c>
-      <c r="E7" s="68"/>
+      <c r="E7" s="69"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="81"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="20"/>
       <c r="E8" s="3"/>
     </row>

</xml_diff>